<commit_message>
Update: Reorganize RSI correlation data and update portfolio analysis
</commit_message>
<xml_diff>
--- a/Pair Trading EA/EURUSD_AUDUSD/EURUSD-AUDUSD.xlsx
+++ b/Pair Trading EA/EURUSD_AUDUSD/EURUSD-AUDUSD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sureshpatil/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sureshpatil/Desktop/Portfolio Creation/Pair Trading EA/EURUSD_AUDUSD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9D5331-A5E2-EA49-927D-17E7B4AC5224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA077BF-9485-9849-AE14-4A7A15835869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="-20980" windowWidth="28040" windowHeight="16640" xr2:uid="{216DC0A2-4271-EC45-92AA-101FBA5B7502}"/>
   </bookViews>
@@ -3185,7 +3185,7 @@
         <v>739</v>
       </c>
       <c r="B1">
-        <v>1086</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>